<commit_message>
fixed #750 FlixelGames-750 アイテム破壊実装
</commit_message>
<xml_diff>
--- a/OneWayRPG/docs/message.xlsx
+++ b/OneWayRPG/docs/message.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="103">
   <si>
     <t>id</t>
   </si>
@@ -211,6 +211,9 @@
   </si>
   <si>
     <t>次のフロアへ進む道を見つけた</t>
+  </si>
+  <si>
+    <t>&lt;val1&gt;は砕け散った</t>
   </si>
   <si>
     <t>攻撃力</t>
@@ -1538,7 +1541,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C57"/>
+  <dimension ref="A1:C58"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1574,7 +1577,7 @@
     </row>
     <row r="3" ht="20" customHeight="1">
       <c r="A3" s="5">
-        <f t="shared" si="0" ref="A3:A57">ROW()-2</f>
+        <f t="shared" si="0" ref="A3:A58">ROW()-2</f>
         <v>1</v>
       </c>
       <c r="B3" t="s" s="4">
@@ -2230,6 +2233,18 @@
       </c>
       <c r="C57" t="s" s="4">
         <v>10</v>
+      </c>
+    </row>
+    <row r="58" ht="20" customHeight="1">
+      <c r="A58" s="5">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="B58" t="s" s="4">
+        <v>66</v>
+      </c>
+      <c r="C58" t="s" s="4">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -2279,7 +2294,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s" s="4">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" ht="20" customHeight="1">
@@ -2288,7 +2303,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s" s="4">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" ht="20" customHeight="1">
@@ -2297,7 +2312,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s" s="4">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" ht="20" customHeight="1">
@@ -2306,7 +2321,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s" s="4">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" ht="20" customHeight="1">
@@ -2315,7 +2330,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s" s="4">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" ht="20" customHeight="1">
@@ -2324,7 +2339,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s" s="4">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" ht="20" customHeight="1">
@@ -2333,7 +2348,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s" s="4">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" ht="20" customHeight="1">
@@ -2342,7 +2357,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s" s="4">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" ht="20" customHeight="1">
@@ -2351,7 +2366,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s" s="4">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12" ht="20" customHeight="1">
@@ -2360,7 +2375,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s" s="4">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" ht="20" customHeight="1">
@@ -2369,7 +2384,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s" s="4">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14" ht="20" customHeight="1">
@@ -2378,7 +2393,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s" s="4">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="15" ht="20" customHeight="1">
@@ -2387,7 +2402,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s" s="4">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="16" ht="20" customHeight="1">
@@ -2396,7 +2411,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s" s="4">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" ht="20" customHeight="1">
@@ -2405,7 +2420,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s" s="4">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18" ht="20" customHeight="1">
@@ -2414,7 +2429,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="s" s="4">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="19" ht="20" customHeight="1">
@@ -2423,7 +2438,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="s" s="4">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="20" ht="20" customHeight="1">
@@ -2432,7 +2447,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="s" s="4">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="21" ht="20" customHeight="1">
@@ -2441,7 +2456,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="s" s="4">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="22" ht="20" customHeight="1">
@@ -2450,7 +2465,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="s" s="4">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="23" ht="20" customHeight="1">
@@ -2459,7 +2474,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="s" s="4">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="24" ht="20" customHeight="1">
@@ -2468,7 +2483,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="s" s="4">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="25" ht="20" customHeight="1">
@@ -2477,7 +2492,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="s" s="4">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="26" ht="20" customHeight="1">
@@ -2486,7 +2501,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="s" s="4">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="27" ht="20" customHeight="1">
@@ -2495,7 +2510,7 @@
         <v>25</v>
       </c>
       <c r="B27" t="s" s="4">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="28" ht="20" customHeight="1">
@@ -2504,7 +2519,7 @@
         <v>26</v>
       </c>
       <c r="B28" t="s" s="4">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="29" ht="20" customHeight="1">
@@ -2513,7 +2528,7 @@
         <v>27</v>
       </c>
       <c r="B29" t="s" s="4">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="30" ht="20" customHeight="1">
@@ -2522,7 +2537,7 @@
         <v>28</v>
       </c>
       <c r="B30" t="s" s="4">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="31" ht="20" customHeight="1">
@@ -2531,7 +2546,7 @@
         <v>29</v>
       </c>
       <c r="B31" t="s" s="4">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="32" ht="20" customHeight="1">
@@ -2540,7 +2555,7 @@
         <v>30</v>
       </c>
       <c r="B32" t="s" s="4">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="33" ht="20" customHeight="1">
@@ -2549,7 +2564,7 @@
         <v>31</v>
       </c>
       <c r="B33" t="s" s="4">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="34" ht="20" customHeight="1">
@@ -2558,7 +2573,7 @@
         <v>32</v>
       </c>
       <c r="B34" t="s" s="4">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="35" ht="20" customHeight="1">
@@ -2567,7 +2582,7 @@
         <v>33</v>
       </c>
       <c r="B35" t="s" s="4">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="36" ht="20" customHeight="1">
@@ -2576,7 +2591,7 @@
         <v>34</v>
       </c>
       <c r="B36" t="s" s="4">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="37" ht="20" customHeight="1">
@@ -2585,7 +2600,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="s" s="4">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="38" ht="20" customHeight="1">
@@ -2594,7 +2609,7 @@
         <v>36</v>
       </c>
       <c r="B38" t="s" s="4">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed #758 FlixelGames-758 歩いた歩数表示
</commit_message>
<xml_diff>
--- a/OneWayRPG/docs/message.xlsx
+++ b/OneWayRPG/docs/message.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="104">
   <si>
     <t>id</t>
   </si>
@@ -214,6 +214,9 @@
   </si>
   <si>
     <t>&lt;val1&gt;は砕け散った</t>
+  </si>
+  <si>
+    <t>食糧を&lt;val1&gt;つ手に入れた</t>
   </si>
   <si>
     <t>攻撃力</t>
@@ -1541,7 +1544,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C58"/>
+  <dimension ref="A1:C59"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1577,7 +1580,7 @@
     </row>
     <row r="3" ht="20" customHeight="1">
       <c r="A3" s="5">
-        <f t="shared" si="0" ref="A3:A58">ROW()-2</f>
+        <f t="shared" si="0" ref="A3:A59">ROW()-2</f>
         <v>1</v>
       </c>
       <c r="B3" t="s" s="4">
@@ -2245,6 +2248,18 @@
       </c>
       <c r="C58" t="s" s="4">
         <v>6</v>
+      </c>
+    </row>
+    <row r="59" ht="20" customHeight="1">
+      <c r="A59" s="5">
+        <f t="shared" si="0"/>
+        <v>57</v>
+      </c>
+      <c r="B59" t="s" s="4">
+        <v>67</v>
+      </c>
+      <c r="C59" t="s" s="4">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -2294,7 +2309,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s" s="4">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" ht="20" customHeight="1">
@@ -2303,7 +2318,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s" s="4">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" ht="20" customHeight="1">
@@ -2312,7 +2327,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s" s="4">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" ht="20" customHeight="1">
@@ -2321,7 +2336,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s" s="4">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" ht="20" customHeight="1">
@@ -2330,7 +2345,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s" s="4">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" ht="20" customHeight="1">
@@ -2339,7 +2354,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s" s="4">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" ht="20" customHeight="1">
@@ -2348,7 +2363,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s" s="4">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" ht="20" customHeight="1">
@@ -2357,7 +2372,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s" s="4">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" ht="20" customHeight="1">
@@ -2366,7 +2381,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s" s="4">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" ht="20" customHeight="1">
@@ -2375,7 +2390,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s" s="4">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13" ht="20" customHeight="1">
@@ -2384,7 +2399,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s" s="4">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" ht="20" customHeight="1">
@@ -2393,7 +2408,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s" s="4">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15" ht="20" customHeight="1">
@@ -2402,7 +2417,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s" s="4">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16" ht="20" customHeight="1">
@@ -2411,7 +2426,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s" s="4">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17" ht="20" customHeight="1">
@@ -2420,7 +2435,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s" s="4">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="18" ht="20" customHeight="1">
@@ -2429,7 +2444,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="s" s="4">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="19" ht="20" customHeight="1">
@@ -2438,7 +2453,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="s" s="4">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="20" ht="20" customHeight="1">
@@ -2447,7 +2462,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="s" s="4">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="21" ht="20" customHeight="1">
@@ -2456,7 +2471,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="s" s="4">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="22" ht="20" customHeight="1">
@@ -2465,7 +2480,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="s" s="4">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="23" ht="20" customHeight="1">
@@ -2474,7 +2489,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="s" s="4">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="24" ht="20" customHeight="1">
@@ -2483,7 +2498,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="s" s="4">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="25" ht="20" customHeight="1">
@@ -2492,7 +2507,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="s" s="4">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="26" ht="20" customHeight="1">
@@ -2501,7 +2516,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="s" s="4">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="27" ht="20" customHeight="1">
@@ -2510,7 +2525,7 @@
         <v>25</v>
       </c>
       <c r="B27" t="s" s="4">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="28" ht="20" customHeight="1">
@@ -2519,7 +2534,7 @@
         <v>26</v>
       </c>
       <c r="B28" t="s" s="4">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="29" ht="20" customHeight="1">
@@ -2528,7 +2543,7 @@
         <v>27</v>
       </c>
       <c r="B29" t="s" s="4">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="30" ht="20" customHeight="1">
@@ -2537,7 +2552,7 @@
         <v>28</v>
       </c>
       <c r="B30" t="s" s="4">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="31" ht="20" customHeight="1">
@@ -2546,7 +2561,7 @@
         <v>29</v>
       </c>
       <c r="B31" t="s" s="4">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="32" ht="20" customHeight="1">
@@ -2555,7 +2570,7 @@
         <v>30</v>
       </c>
       <c r="B32" t="s" s="4">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="33" ht="20" customHeight="1">
@@ -2564,7 +2579,7 @@
         <v>31</v>
       </c>
       <c r="B33" t="s" s="4">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="34" ht="20" customHeight="1">
@@ -2573,7 +2588,7 @@
         <v>32</v>
       </c>
       <c r="B34" t="s" s="4">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="35" ht="20" customHeight="1">
@@ -2582,7 +2597,7 @@
         <v>33</v>
       </c>
       <c r="B35" t="s" s="4">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="36" ht="20" customHeight="1">
@@ -2591,7 +2606,7 @@
         <v>34</v>
       </c>
       <c r="B36" t="s" s="4">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="37" ht="20" customHeight="1">
@@ -2600,7 +2615,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="s" s="4">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="38" ht="20" customHeight="1">
@@ -2609,7 +2624,7 @@
         <v>36</v>
       </c>
       <c r="B38" t="s" s="4">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>